<commit_message>
Fixed so many errors
</commit_message>
<xml_diff>
--- a/biz_coded.xlsx
+++ b/biz_coded.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ESRI_MAPINFO_SHEET" sheetId="2" state="veryHidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ESRI_MAPINFO_SHEET" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>business name</t>
   </si>
@@ -33,6 +34,30 @@
   </si>
   <si>
     <t>541618</t>
+  </si>
+  <si>
+    <t>fakeco</t>
+  </si>
+  <si>
+    <t>NOT FOUND</t>
+  </si>
+  <si>
+    <t>green lantern lounge</t>
+  </si>
+  <si>
+    <t>722511</t>
+  </si>
+  <si>
+    <t>leo’s country oven</t>
+  </si>
+  <si>
+    <t>thang long</t>
+  </si>
+  <si>
+    <t>galco</t>
+  </si>
+  <si>
+    <t>443142</t>
   </si>
 </sst>
 </file>
@@ -40,13 +65,34 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Verdana"/>
+      <family val="0"/>
+      <b val="1"/>
+      <sz val="50"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,16 +112,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -154,7 +215,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -189,7 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -366,65 +425,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="14.28515625"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="10.7109375"/>
+    <col customWidth="1" max="1" min="1" style="1" width="14.28"/>
+    <col customWidth="1" max="2" min="2" style="1" width="10.71"/>
+    <col customWidth="1" max="1025" min="3" style="1" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row customHeight="1" ht="15" r="1" s="2" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row customHeight="1" ht="15" r="2" s="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row customHeight="1" ht="15" r="3" s="2" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
+    <row customHeight="1" ht="13.8" r="4" s="2" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="5" s="2" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="6" s="2" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="7" s="2" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="8" s="2" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.67"/>
+  </cols>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>